<commit_message>
correlation analysis of metric1&2&6 and metric5&6.
</commit_message>
<xml_diff>
--- a/data analysis/Correction 5&6/dataAnalysisOf5&6.xlsx
+++ b/data analysis/Correction 5&6/dataAnalysisOf5&6.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/study/master/19winter/soen6611/Metrics-Correlation-Analysis/data analysis/Correction 5&amp;6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF5A83ED-3AA6-E44A-B4EA-AED1F755C790}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE90980C-A5A3-B142-8AEB-DB6E3BB09514}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5280" yWindow="1860" windowWidth="20120" windowHeight="12280" xr2:uid="{E33041DE-B5BD-FB41-8560-4F060210710A}"/>
+    <workbookView xWindow="14900" yWindow="5160" windowWidth="20120" windowHeight="12280" xr2:uid="{E33041DE-B5BD-FB41-8560-4F060210710A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -467,7 +467,7 @@
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -497,7 +497,7 @@
         <v>10.833</v>
       </c>
       <c r="C2">
-        <v>788588</v>
+        <v>5.9171597633136076E-3</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -508,7 +508,7 @@
         <v>43.332999999999998</v>
       </c>
       <c r="C3">
-        <v>795044</v>
+        <v>2.0833333333333343E-2</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -519,7 +519,7 @@
         <v>33.968299999999999</v>
       </c>
       <c r="C4">
-        <v>805117</v>
+        <v>1.7241379310344838E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -530,7 +530,7 @@
         <v>30.555599999999998</v>
       </c>
       <c r="C5">
-        <v>163928</v>
+        <v>3.125E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -541,7 +541,7 @@
         <v>44.444400000000002</v>
       </c>
       <c r="C6">
-        <v>167571</v>
+        <v>4.1666666666666678E-2</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -552,7 +552,7 @@
         <v>100</v>
       </c>
       <c r="C7">
-        <v>141893</v>
+        <v>2.5641025641025637E-2</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -563,7 +563,7 @@
         <v>40.317500000000003</v>
       </c>
       <c r="C8">
-        <v>881736</v>
+        <v>1.7730496453900704E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -574,7 +574,7 @@
         <v>38.611000000000004</v>
       </c>
       <c r="C9">
-        <v>914516</v>
+        <v>5.0761421319796924E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -585,7 +585,7 @@
         <v>41.666699999999999</v>
       </c>
       <c r="C10">
-        <v>943754</v>
+        <v>3.0303030303030294E-3</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -596,7 +596,7 @@
         <v>66.667000000000002</v>
       </c>
       <c r="C11">
-        <v>698588</v>
+        <v>9.9009900990099167E-3</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -607,7 +607,7 @@
         <v>15.7576</v>
       </c>
       <c r="C12">
-        <v>610800</v>
+        <v>7.1428571428571425E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -618,7 +618,7 @@
         <v>3.0303</v>
       </c>
       <c r="C13">
-        <v>722335</v>
+        <v>5.2356020942408415E-3</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -629,7 +629,7 @@
         <v>250</v>
       </c>
       <c r="C14">
-        <v>691089</v>
+        <v>4.5454545454545449E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -640,7 +640,7 @@
         <v>66.667000000000002</v>
       </c>
       <c r="C15">
-        <v>842107</v>
+        <v>7.7041602465331151E-4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>